<commit_message>
TD-5119  Bulk uploads are not validating the values of the fields that depend on the value of another field
</commit_message>
<xml_diff>
--- a/test/fixtures/upload_invalid_hierarchy.xlsx
+++ b/test/fixtures/upload_invalid_hierarchy.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
   <si>
     <t>name</t>
   </si>
@@ -40,6 +40,12 @@
     <t>hierarchy_name_2</t>
   </si>
   <si>
+    <t>father</t>
+  </si>
+  <si>
+    <t>son</t>
+  </si>
+  <si>
     <t>domain</t>
   </si>
   <si>
@@ -55,13 +61,16 @@
     <t>Role</t>
   </si>
   <si>
-    <t>error</t>
-  </si>
-  <si>
     <t>children_2</t>
   </si>
   <si>
     <t>children_2|children_2</t>
+  </si>
+  <si>
+    <t>a1</t>
+  </si>
+  <si>
+    <t>b11</t>
   </si>
 </sst>
 </file>
@@ -79,7 +88,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF000000"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -117,10 +126,10 @@
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="general"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="general"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -424,7 +433,7 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
@@ -437,10 +446,12 @@
     <col min="5" max="5" style="3" width="11.862142857142858" customWidth="1" bestFit="1"/>
     <col min="6" max="6" style="3" width="17.433571428571426" customWidth="1" bestFit="1"/>
     <col min="7" max="7" style="3" width="20.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="3" width="11.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="3" width="20.14785714285714" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="3" width="11.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="3" width="11.862142857142858" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="16.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -465,57 +476,43 @@
       <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="I1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="16.5">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="C2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="D2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="E2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="H2" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
-      <c r="A3" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G3" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>15</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>